<commit_message>
Cambios en el 2. para juli
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\Github\VEN\data_management\management\4. income imputation\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F84D8C-D69D-4EB8-AAFD-08411649D74E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -64,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -105,18 +111,26 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,25 +430,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="true"/>
-    <col min="2" max="3" width="14.33203125" customWidth="true"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="3" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3">
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
@@ -442,7 +456,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="28.8">
+    <row r="4" spans="1:3" ht="28.8">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -450,16 +464,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="4">
-        <v>0.049594974375929905</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>0.048034584901128809</v>
-      </c>
-    </row>
-    <row r="5" ht="28.8">
+        <v>4.9594974375929905E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -469,14 +477,8 @@
       <c r="C5" s="4">
         <v>30.781947429327161</v>
       </c>
-      <c r="D5">
-        <v>3837</v>
-      </c>
-      <c r="E5">
-        <v>30.718117044271875</v>
-      </c>
-    </row>
-    <row r="6" ht="28.8">
+    </row>
+    <row r="6" spans="1:3" ht="28.8">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -486,14 +488,8 @@
       <c r="C6" s="4">
         <v>8.6873863448503883</v>
       </c>
-      <c r="D6">
-        <v>1090</v>
-      </c>
-      <c r="E6">
-        <v>8.7262829237050674</v>
-      </c>
-    </row>
-    <row r="7" ht="28.8">
+    </row>
+    <row r="7" spans="1:3" ht="28.8">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -503,14 +499,8 @@
       <c r="C7" s="4">
         <v>39.469333774177549</v>
       </c>
-      <c r="D7">
-        <v>4927</v>
-      </c>
-      <c r="E7">
-        <v>39.444399967976942</v>
-      </c>
-    </row>
-    <row r="8">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -520,14 +510,8 @@
       <c r="C8" s="4">
         <v>60.481071251446515</v>
       </c>
-      <c r="D8">
-        <v>7559</v>
-      </c>
-      <c r="E8">
-        <v>60.51557121127211</v>
-      </c>
-    </row>
-    <row r="9">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -537,26 +521,20 @@
       <c r="C9" s="4">
         <v>100</v>
       </c>
-      <c r="D9">
-        <v>12491</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10">
+    </row>
+    <row r="10" spans="1:3">
       <c r="C10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3">
       <c r="C11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -564,7 +542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" ht="28.8">
+    <row r="14" spans="1:3" ht="28.8">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -574,14 +552,8 @@
       <c r="C14" s="4">
         <v>372.25641025641028</v>
       </c>
-      <c r="D14">
-        <v>22500</v>
-      </c>
-      <c r="E14">
-        <v>372.27001985440108</v>
-      </c>
-    </row>
-    <row r="15" ht="28.8">
+    </row>
+    <row r="15" spans="1:3" ht="28.8">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -591,14 +563,8 @@
       <c r="C15" s="4">
         <v>0.30769230769230771</v>
       </c>
-      <c r="D15">
-        <v>18</v>
-      </c>
-      <c r="E15">
-        <v>0.29781601588352086</v>
-      </c>
-    </row>
-    <row r="16" ht="43.2">
+    </row>
+    <row r="16" spans="1:3" ht="43.2">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -608,14 +574,8 @@
       <c r="C16" s="4">
         <v>0.29059829059829062</v>
       </c>
-      <c r="D16">
-        <v>17</v>
-      </c>
-      <c r="E16">
-        <v>0.2812706816677697</v>
-      </c>
-    </row>
-    <row r="17">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -625,14 +585,8 @@
       <c r="C17" s="4">
         <v>0.59829059829059839</v>
       </c>
-      <c r="D17">
-        <v>35</v>
-      </c>
-      <c r="E17">
-        <v>0.5790866975512905</v>
-      </c>
-    </row>
-    <row r="18">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -642,14 +596,8 @@
       <c r="C18" s="4">
         <v>99.025641025641022</v>
       </c>
-      <c r="D18">
-        <v>5986</v>
-      </c>
-      <c r="E18">
-        <v>99.040370615486424</v>
-      </c>
-    </row>
-    <row r="19" ht="28.8">
+    </row>
+    <row r="19" spans="1:3" ht="28.8">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -657,12 +605,6 @@
         <v>5850</v>
       </c>
       <c r="C19" s="4">
-        <v>100</v>
-      </c>
-      <c r="D19">
-        <v>6044</v>
-      </c>
-      <c r="E19">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1° version imputación laboral monetario
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,29 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\Github\VEN\data_management\management\4. income imputation\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F84D8C-D69D-4EB8-AAFD-08411649D74E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D182B799-150E-4AF8-B3F2-FB88CD8A69E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
+    <sheet name="labor_incmon_imp_stochastic_reg" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>Real zeros (answered 0 or said didn't receive income)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Missing values: Occupied, but didn't answer if received ila</t>
   </si>
   <si>
-    <t>Missing values: said received monetary ila, but amount missing</t>
-  </si>
-  <si>
     <t>Missing values: Total missing (sum both cases)</t>
   </si>
   <si>
@@ -40,38 +35,98 @@
     <t>Total employed, or receive ila mon</t>
   </si>
   <si>
-    <t>Labor income</t>
-  </si>
-  <si>
-    <t>Pensions</t>
-  </si>
-  <si>
-    <t>Zeros (answered 0 or said didn't receive pension)</t>
-  </si>
-  <si>
-    <t>Missing values: Those who replied they do not know if they received pensions</t>
-  </si>
-  <si>
-    <t>Missing values: Those who replied they received pensions but they did not declare the amount</t>
-  </si>
-  <si>
     <t>Total missing values</t>
   </si>
   <si>
     <t>All pensioners and retired, or receive pension/retirement benefits</t>
   </si>
   <si>
+    <t>Missing values: Said received monetary ila, but amount missing</t>
+  </si>
+  <si>
+    <t>Real zeros: Answered 0 or said didn't receive income</t>
+  </si>
+  <si>
+    <t>Monetary labor income</t>
+  </si>
+  <si>
+    <t>Pensions and retirement benefits, non-labor income</t>
+  </si>
+  <si>
+    <t>Real zeros (answered 0 or said didn't receive pension)</t>
+  </si>
+  <si>
+    <t>Missing values: Said received pension, but amount missing</t>
+  </si>
+  <si>
+    <t>Missing values: Jubilado/Pensionado, but didn't answer if received pension</t>
+  </si>
+  <si>
+    <t>Monetary non-labor income (all except pensions)</t>
+  </si>
+  <si>
+    <t>Obs.</t>
+  </si>
+  <si>
     <t>Percentage</t>
   </si>
   <si>
-    <t>Obs.</t>
+    <t>Missing values: Said received monetary non-labor income, but amount missing</t>
+  </si>
+  <si>
+    <t>All receiving non-monetary labor income</t>
+  </si>
+  <si>
+    <t>Non-monetary labor income</t>
+  </si>
+  <si>
+    <t>Zeros: answered 0 or said didn't receive non-monetary labor income</t>
+  </si>
+  <si>
+    <t>Real zeros: answered 0 or said didn't receive monetary non-labor income</t>
+  </si>
+  <si>
+    <t>Missing values: Said received non-monetary ila, but amount missing</t>
+  </si>
+  <si>
+    <t>Note: values to impute in yellow.</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>p10</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p50</t>
+  </si>
+  <si>
+    <t>p75</t>
+  </si>
+  <si>
+    <t>p90</t>
+  </si>
+  <si>
+    <t>Without imputing missing values</t>
+  </si>
+  <si>
+    <t>Imputing missing values</t>
+  </si>
+  <si>
+    <t>All receiving monetary non-labor income</t>
+  </si>
+  <si>
+    <t>ila_monetario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -88,16 +143,42 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,18 +186,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,6 +251,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC021AF-7E78-4D5A-AE56-D358923A848E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1097280"/>
+          <a:ext cx="5120640" cy="3749040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,184 +616,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C19"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.21875" customWidth="true"/>
-    <col min="2" max="3" width="14.33203125" customWidth="true"/>
+    <col min="1" max="1" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:3">
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="9">
+        <v>4.9594974375929905E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
+        <v>193</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1.5953050090924119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3724</v>
+      </c>
+      <c r="C6" s="9">
+        <v>30.781947429327161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3917</v>
+      </c>
+      <c r="C7" s="9">
+        <v>32.377252438419575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <v>8113</v>
+      </c>
+      <c r="C8" s="9">
+        <v>67.06067118531989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="13">
+        <v>12098</v>
+      </c>
+      <c r="C9" s="14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="28.8">
+      <c r="A14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11">
+        <v>57</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.96839959225280325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8">
+      <c r="A15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="8">
+        <v>7</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.11892626571525654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8">
+      <c r="A16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8">
+        <v>18</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.3058103975535168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="10">
+        <v>25</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.42473666326877335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="8">
+        <v>5804</v>
+      </c>
+      <c r="C18" s="9">
+        <v>98.606863744478417</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" ht="28.8">
+      <c r="A19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="13">
+        <v>5886</v>
+      </c>
+      <c r="C19" s="14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" ht="28.8">
+      <c r="A24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="8">
+        <v>15</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1.8382352941176472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8">
+      <c r="A25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="10">
+        <v>16</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1.9607843137254901</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8">
+        <v>785</v>
+      </c>
+      <c r="C26" s="9">
+        <v>96.200980392156865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="13">
+        <v>816</v>
+      </c>
+      <c r="C27" s="14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" ht="28.8">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.049594974375929905</v>
-      </c>
-    </row>
-    <row r="5" ht="28.8">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>3724</v>
-      </c>
-      <c r="C5" s="4">
-        <v>30.781947429327161</v>
-      </c>
-    </row>
-    <row r="6" ht="28.8">
-      <c r="A6" s="3" t="s">
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" ht="28.8">
+      <c r="A32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="8">
+        <v>3</v>
+      </c>
+      <c r="C32" s="9">
+        <v>5.152868430092751E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8">
+      <c r="A33" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="10">
+        <v>43</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.73857780831329445</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>193</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.5953050090924119</v>
-      </c>
-    </row>
-    <row r="7" ht="28.8">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>3917</v>
-      </c>
-      <c r="C7" s="4">
-        <v>32.377252438419575</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>8155</v>
-      </c>
-      <c r="C8" s="4">
-        <v>67.407836005951395</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>12098</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B34" s="8">
+        <v>5775</v>
+      </c>
+      <c r="C34" s="9">
+        <v>99.192717279285475</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.8">
+      <c r="A35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="13">
+        <v>5822</v>
+      </c>
+      <c r="C35" s="14">
         <v>100</v>
       </c>
     </row>
-    <row r="10">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" ht="28.8">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>21777</v>
-      </c>
-      <c r="C14" s="4">
-        <v>372.25641025641028</v>
-      </c>
-    </row>
-    <row r="15" ht="28.8">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.30769230769230771</v>
-      </c>
-    </row>
-    <row r="16" ht="43.2">
-      <c r="A16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.11965811965811966</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.42735042735042739</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>5804</v>
-      </c>
-      <c r="C18" s="4">
-        <v>99.213675213675216</v>
-      </c>
-    </row>
-    <row r="19" ht="28.8">
-      <c r="A19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19">
-        <v>5850</v>
-      </c>
-      <c r="C19" s="4">
-        <v>100</v>
+    <row r="37" spans="1:3">
+      <c r="A37" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>6481537819.878829</v>
+      </c>
+      <c r="C4">
+        <v>333333.34375</v>
+      </c>
+      <c r="D4">
+        <v>700000</v>
+      </c>
+      <c r="E4">
+        <v>1500000</v>
+      </c>
+      <c r="F4">
+        <v>3229734.5</v>
+      </c>
+      <c r="G4">
+        <v>6000000</v>
+      </c>
+      <c r="H4">
+        <v>4372125194.1933126</v>
+      </c>
+      <c r="I4">
+        <v>416666.65625</v>
+      </c>
+      <c r="J4">
+        <v>794301.625</v>
+      </c>
+      <c r="K4">
+        <v>1634120.125</v>
+      </c>
+      <c r="L4">
+        <v>3303803.75</v>
+      </c>
+      <c r="M4">
+        <v>6025734.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Imputed mon labor inc. + corrections ENCOVI2019
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Missing values: Occupied, but didn't answer if received ila</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>All receiving monetary non-labor income</t>
-  </si>
-  <si>
-    <t>ila_monetario</t>
   </si>
   <si>
     <t>2019</t>
@@ -246,23 +243,23 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC021AF-7E78-4D5A-AE56-D358923A848E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0599746E-3476-44B6-954C-DABB308F7A6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -285,7 +282,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="609600" y="1097280"/>
+          <a:off x="1485900" y="1021080"/>
           <a:ext cx="5120640" cy="3749040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -605,13 +602,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -619,7 +616,7 @@
     <col min="1" max="1" width="34.21875" customWidth="true"/>
     <col min="2" max="2" width="11.88671875" customWidth="true"/>
     <col min="3" max="3" width="10.77734375" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="5.5546875" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="5" bestFit="true" customWidth="true"/>
     <col min="5" max="5" width="12" bestFit="true" customWidth="true"/>
     <col min="6" max="6" width="5" bestFit="true" customWidth="true"/>
     <col min="7" max="7" width="12" bestFit="true" customWidth="true"/>
@@ -631,8 +628,6 @@
     <col min="13" max="13" width="12" bestFit="true" customWidth="true"/>
     <col min="14" max="14" width="5" bestFit="true" customWidth="true"/>
     <col min="15" max="15" width="12" bestFit="true" customWidth="true"/>
-    <col min="16" max="16" width="5" bestFit="true" customWidth="true"/>
-    <col min="17" max="17" width="12" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -675,10 +670,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="8">
-        <v>3724</v>
+        <v>3726</v>
       </c>
       <c r="C6" s="9">
-        <v>30.781947429327161</v>
+        <v>30.798479087452474</v>
       </c>
     </row>
     <row r="7" ht="28.8">
@@ -686,10 +681,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="10">
-        <v>3917</v>
+        <v>3919</v>
       </c>
       <c r="C7" s="9">
-        <v>32.377252438419575</v>
+        <v>32.393784096544884</v>
       </c>
     </row>
     <row r="8">
@@ -697,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="8">
-        <v>8113</v>
+        <v>8142</v>
       </c>
       <c r="C8" s="9">
-        <v>67.06067118531989</v>
+        <v>67.300380228136873</v>
       </c>
     </row>
     <row r="9">
@@ -783,7 +778,6 @@
       <c r="C18" s="9">
         <v>98.606863744478417</v>
       </c>
-      <c r="D18" s="6"/>
     </row>
     <row r="19" ht="28.8">
       <c r="A19" s="12" t="s">
@@ -931,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -956,9 +950,6 @@
       <c r="M1" s="17"/>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>2019</v>
-      </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
@@ -998,10 +989,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <v>6481537819.878829</v>
+        <v>6416995775.2467194</v>
       </c>
       <c r="C4">
         <v>333333.34375</v>
@@ -1013,28 +1004,28 @@
         <v>1500000</v>
       </c>
       <c r="F4">
-        <v>3229734.5</v>
+        <v>3203803.75</v>
       </c>
       <c r="G4">
         <v>6000000</v>
       </c>
       <c r="H4">
-        <v>4372124178.3203964</v>
+        <v>4332936007.9559231</v>
       </c>
       <c r="I4">
-        <v>416666.65625</v>
+        <v>185559.5625</v>
       </c>
       <c r="J4">
-        <v>796253.875</v>
+        <v>600000</v>
       </c>
       <c r="K4">
-        <v>1632763.375</v>
+        <v>1250000</v>
       </c>
       <c r="L4">
-        <v>3300000</v>
+        <v>3103803.75</v>
       </c>
       <c r="M4">
-        <v>6037799.25</v>
+        <v>6178718.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando income indep a la imputación y los outliers a las 2 imp que faltaban
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -1,74 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb550905\Github\VEN\data_management\management\4. income imputation\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F84D8C-D69D-4EB8-AAFD-08411649D74E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="9336" yWindow="4260" windowWidth="17280" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
-    <sheet name="labor_jubpenimp_stochastic_reg" sheetId="2" r:id="rId5"/>
+    <sheet name="labor_incmon_imp_stochastic_reg" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
-  <si>
-    <t>Real zeros (answered 0 or said didn't receive income)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Missing values: Occupied, but didn't answer if received ila</t>
   </si>
   <si>
-    <t>Missing values: said received monetary ila, but amount missing</t>
-  </si>
-  <si>
-    <t>Missing values: Total missing (sum both cases)</t>
-  </si>
-  <si>
     <t>Non-zero values</t>
   </si>
   <si>
     <t>Total employed, or receive ila mon</t>
   </si>
   <si>
-    <t>Labor income</t>
-  </si>
-  <si>
-    <t>Pensions</t>
-  </si>
-  <si>
-    <t>Zeros (answered 0 or said didn't receive pension)</t>
-  </si>
-  <si>
-    <t>Missing values: Those who replied they do not know if they received pensions</t>
-  </si>
-  <si>
-    <t>Missing values: Those who replied they received pensions but they did not declare the amount</t>
-  </si>
-  <si>
-    <t>Total missing values</t>
-  </si>
-  <si>
     <t>All pensioners and retired, or receive pension/retirement benefits</t>
   </si>
   <si>
+    <t>Missing values: Said received monetary ila, but amount missing</t>
+  </si>
+  <si>
+    <t>Real zeros: Answered 0 or said didn't receive income</t>
+  </si>
+  <si>
+    <t>Monetary labor income</t>
+  </si>
+  <si>
+    <t>Pensions and retirement benefits, non-labor income</t>
+  </si>
+  <si>
+    <t>Real zeros (answered 0 or said didn't receive pension)</t>
+  </si>
+  <si>
+    <t>Missing values: Said received pension, but amount missing</t>
+  </si>
+  <si>
+    <t>Missing values: Jubilado/Pensionado, but didn't answer if received pension</t>
+  </si>
+  <si>
+    <t>Monetary non-labor income (all except pensions)</t>
+  </si>
+  <si>
+    <t>Obs.</t>
+  </si>
+  <si>
     <t>Percentage</t>
   </si>
   <si>
-    <t>Obs.</t>
-  </si>
-  <si>
-    <t>2019</t>
+    <t>Missing values: Said received monetary non-labor income, but amount missing</t>
+  </si>
+  <si>
+    <t>All receiving non-monetary labor income</t>
+  </si>
+  <si>
+    <t>Non-monetary labor income</t>
+  </si>
+  <si>
+    <t>Real zeros: answered 0 or said didn't receive monetary non-labor income</t>
+  </si>
+  <si>
+    <t>Missing values: Said received non-monetary ila, but amount missing</t>
+  </si>
+  <si>
+    <t>Note: values to impute in yellow.</t>
   </si>
   <si>
     <t>mean</t>
@@ -87,13 +93,37 @@
   </si>
   <si>
     <t>p90</t>
+  </si>
+  <si>
+    <t>Without imputing missing values</t>
+  </si>
+  <si>
+    <t>Imputing missing values</t>
+  </si>
+  <si>
+    <t>All receiving monetary non-labor income</t>
+  </si>
+  <si>
+    <t>ila_monetario</t>
+  </si>
+  <si>
+    <t>Missing values: outliers</t>
+  </si>
+  <si>
+    <t>Total missing (sum the three cases)</t>
+  </si>
+  <si>
+    <t>Total missing (sum of both cases)</t>
+  </si>
+  <si>
+    <t>Real zeros: answered 0 or said didn't receive non-monetary labor income</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -110,16 +140,42 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,33 +183,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC021AF-7E78-4D5A-AE56-D358923A848E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true" noChangeArrowheads="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1097280"/>
+          <a:ext cx="5120640" cy="3749040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,273 +601,525 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="34.21875" customWidth="true"/>
-    <col min="2" max="3" width="14.33203125" customWidth="true"/>
+    <col min="2" max="2" width="11.88671875" customWidth="true"/>
+    <col min="3" max="3" width="10.77734375" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.5546875" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="12" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="5" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="5" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="5" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="12" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="5" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="12" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="5" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="12" bestFit="true" customWidth="true"/>
+    <col min="16" max="16" width="5" bestFit="true" customWidth="true"/>
+    <col min="17" max="17" width="12" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="4" ht="28.8">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>168</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1.3886592825260373</v>
+      </c>
+    </row>
+    <row r="5" ht="28.8">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>621</v>
+      </c>
+      <c r="C5" s="7">
+        <v>5.1330798479087454</v>
+      </c>
+    </row>
+    <row r="6" ht="28.8">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.049594974375929905</v>
-      </c>
-    </row>
-    <row r="5" ht="28.8">
-      <c r="A5" s="3" t="s">
+      <c r="B6" s="6">
+        <v>1540</v>
+      </c>
+      <c r="C6" s="7">
+        <v>12.729376756488675</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6">
+        <v>43</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.35543064969416432</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2204</v>
+      </c>
+      <c r="C8" s="7">
+        <v>18.217887254091586</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>3724</v>
-      </c>
-      <c r="C5" s="4">
-        <v>30.781947429327161</v>
-      </c>
-    </row>
-    <row r="6" ht="28.8">
-      <c r="A6" s="3" t="s">
+      <c r="B9" s="6">
+        <v>9693</v>
+      </c>
+      <c r="C9" s="7">
+        <v>80.120681104314755</v>
+      </c>
+      <c r="D9" s="4">
+        <f>SUM(C8:C9,C4)</f>
+        <v>99.727227640932384</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>193</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1.5953050090924119</v>
-      </c>
-    </row>
-    <row r="7" ht="28.8">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>3917</v>
-      </c>
-      <c r="C7" s="4">
-        <v>32.377252438419575</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>8155</v>
-      </c>
-      <c r="C8" s="4">
-        <v>67.407836005951395</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
+      <c r="B10" s="11">
         <v>12098</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="12">
         <v>100</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11">
       <c r="C11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" ht="28.8">
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="9">
+        <v>57</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.96839959225280325</v>
+      </c>
+    </row>
+    <row r="16" ht="28.8">
+      <c r="A16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6">
+        <v>147</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2.4974515800203876</v>
+      </c>
+    </row>
+    <row r="17" ht="28.8">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.3058103975535168</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="6">
+        <v>7</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.11892626571525654</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="8">
+        <v>172</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2.9221882432891606</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6">
+        <v>5657</v>
+      </c>
+      <c r="C20" s="7">
+        <v>96.109412164458035</v>
+      </c>
+      <c r="D20" s="4">
+        <f>SUM(C19:C20,C15)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" ht="28.8">
+      <c r="A21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="11">
+        <v>5886</v>
+      </c>
+      <c r="C21" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23">
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" ht="28.8">
+      <c r="A26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="15">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1.8382352941176472</v>
+      </c>
+    </row>
+    <row r="27" ht="28.8">
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="15">
+        <v>55</v>
+      </c>
+      <c r="C27" s="7">
+        <v>6.7401960784313726</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="15">
+        <v>2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.24509803921568626</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="8">
+        <v>57</v>
+      </c>
+      <c r="C29" s="7">
+        <v>6.9852941176470589</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6">
+        <v>744</v>
+      </c>
+      <c r="C30" s="7">
+        <v>91.17647058823529</v>
+      </c>
+      <c r="D30" s="4">
+        <f>SUM(C29:C30,C26)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="11">
+        <v>816</v>
+      </c>
+      <c r="C31" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33">
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35">
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" ht="28.8">
+      <c r="A36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="6">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0.05152868430092751</v>
+      </c>
+    </row>
+    <row r="37" ht="28.8">
+      <c r="A37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" ht="28.8">
-      <c r="A14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>21777</v>
-      </c>
-      <c r="C14" s="4">
-        <v>372.25641025641028</v>
-      </c>
-    </row>
-    <row r="15" ht="28.8">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.30769230769230771</v>
-      </c>
-    </row>
-    <row r="16" ht="43.2">
-      <c r="A16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.11965811965811966</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.42735042735042739</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>5804</v>
-      </c>
-      <c r="C18" s="4">
-        <v>99.213675213675216</v>
-      </c>
-    </row>
-    <row r="19" ht="28.8">
-      <c r="A19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19">
-        <v>5850</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B37" s="15">
+        <v>155</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2.6623153555479218</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="15">
+        <v>66</v>
+      </c>
+      <c r="C38" s="7">
+        <v>1.1336310546204054</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="8">
+        <v>221</v>
+      </c>
+      <c r="C39" s="7">
+        <v>3.7959464101683271</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="6">
+        <v>5597</v>
+      </c>
+      <c r="C40" s="7">
+        <v>96.135348677430429</v>
+      </c>
+      <c r="D40" s="4">
+        <f>SUM(C39:C40,C36)</f>
+        <v>98.84919271727928</v>
+      </c>
+    </row>
+    <row r="41" ht="28.8">
+      <c r="A41" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="11">
+        <v>5822</v>
+      </c>
+      <c r="C41" s="12">
         <v>100</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:M4"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
+    <row r="1">
+      <c r="B1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+    </row>
     <row r="3">
+      <c r="A3">
+        <v>2019</v>
+      </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>10986152.731503172</v>
+        <v>6481537819.878829</v>
       </c>
       <c r="C4">
-        <v>250000</v>
+        <v>333333.34375</v>
       </c>
       <c r="D4">
-        <v>250000</v>
+        <v>700000</v>
       </c>
       <c r="E4">
-        <v>2203803.75</v>
+        <v>1500000</v>
       </c>
       <c r="F4">
-        <v>2453803.75</v>
+        <v>3229734.5</v>
       </c>
       <c r="G4">
-        <v>2553803.75</v>
+        <v>6000000</v>
       </c>
       <c r="H4">
-        <v>10952261.519262988</v>
+        <v>4372125194.1933126</v>
       </c>
       <c r="I4">
-        <v>250000</v>
+        <v>416666.65625</v>
       </c>
       <c r="J4">
-        <v>250000</v>
+        <v>794301.625</v>
       </c>
       <c r="K4">
-        <v>2203803.75</v>
+        <v>1634120.125</v>
       </c>
       <c r="L4">
-        <v>2453803.75</v>
+        <v>3303803.75</v>
       </c>
       <c r="M4">
-        <v>2553803.75</v>
+        <v>6025734.75</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en Do Imputation
Do 1, 2 y 4
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -258,7 +258,7 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+            <a:ext xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC021AF-7E78-4D5A-AE56-D358923A848E}"/>
             </a:ext>
           </a:extLst>
@@ -270,7 +270,7 @@
       <xdr:blipFill>
         <a:blip r:embed="rId1" cstate="print">
           <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+            <a:ext xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
@@ -290,7 +290,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>

</xml_diff>

<commit_message>
Corrección todos los ingresos y TC
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -258,7 +258,7 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
-            <a:ext xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC021AF-7E78-4D5A-AE56-D358923A848E}"/>
             </a:ext>
           </a:extLst>
@@ -270,7 +270,7 @@
       <xdr:blipFill>
         <a:blip r:embed="rId1" cstate="print">
           <a:extLst>
-            <a:ext xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
@@ -290,7 +290,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -683,10 +683,10 @@
         <v>30</v>
       </c>
       <c r="B7" s="6">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7">
-        <v>0.35543064969416432</v>
+        <v>0.29756984625557942</v>
       </c>
     </row>
     <row r="8">
@@ -694,10 +694,10 @@
         <v>31</v>
       </c>
       <c r="B8" s="8">
-        <v>2204</v>
+        <v>2197</v>
       </c>
       <c r="C8" s="7">
-        <v>18.217887254091586</v>
+        <v>18.160026450653</v>
       </c>
     </row>
     <row r="9">
@@ -705,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="6">
-        <v>9693</v>
+        <v>9700</v>
       </c>
       <c r="C9" s="7">
-        <v>80.120681104314755</v>
+        <v>80.178541907753342</v>
       </c>
       <c r="D9" s="4">
         <f>SUM(C8:C9,C4)</f>
@@ -780,10 +780,10 @@
         <v>30</v>
       </c>
       <c r="B18" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="7">
-        <v>0.11892626571525654</v>
+        <v>0.10193679918450561</v>
       </c>
     </row>
     <row r="19">
@@ -791,10 +791,10 @@
         <v>31</v>
       </c>
       <c r="B19" s="8">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" s="7">
-        <v>2.9221882432891606</v>
+        <v>2.90519877675841</v>
       </c>
     </row>
     <row r="20">
@@ -802,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="6">
-        <v>5657</v>
+        <v>5658</v>
       </c>
       <c r="C20" s="7">
-        <v>96.109412164458035</v>
+        <v>96.126401630988795</v>
       </c>
       <c r="D20" s="4">
         <f>SUM(C19:C20,C15)</f>
@@ -950,10 +950,10 @@
         <v>30</v>
       </c>
       <c r="B38" s="15">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C38" s="7">
-        <v>1.1336310546204054</v>
+        <v>1.4771556166265889</v>
       </c>
     </row>
     <row r="39">
@@ -961,10 +961,10 @@
         <v>32</v>
       </c>
       <c r="B39" s="8">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C39" s="7">
-        <v>3.7959464101683271</v>
+        <v>4.13947097217451</v>
       </c>
     </row>
     <row r="40">
@@ -972,10 +972,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="6">
-        <v>5597</v>
+        <v>5577</v>
       </c>
       <c r="C40" s="7">
-        <v>96.135348677430429</v>
+        <v>95.791824115424248</v>
       </c>
       <c r="D40" s="4">
         <f>SUM(C39:C40,C36)</f>

</xml_diff>

<commit_message>
Imputaciones de ila_m y inla no jub
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_MA.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="missing_values" sheetId="1" r:id="rId1"/>
     <sheet name="labor_incmon_imp_stochastic_reg" sheetId="2" r:id="rId2"/>
+    <sheet name="nonlabor_imp_stochastic_reg" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Missing values: Occupied, but didn't answer if received ila</t>
   </si>
@@ -117,6 +118,12 @@
   </si>
   <si>
     <t>Real zeros: answered 0 or said didn't receive non-monetary labor income</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>p99</t>
   </si>
 </sst>
 </file>
@@ -683,10 +690,10 @@
         <v>30</v>
       </c>
       <c r="B7" s="6">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7">
-        <v>0.29756984625557942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -694,10 +701,10 @@
         <v>31</v>
       </c>
       <c r="B8" s="8">
-        <v>2197</v>
+        <v>2161</v>
       </c>
       <c r="C8" s="7">
-        <v>18.160026450653</v>
+        <v>17.862456604397419</v>
       </c>
     </row>
     <row r="9">
@@ -780,10 +787,10 @@
         <v>30</v>
       </c>
       <c r="B18" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C18" s="7">
-        <v>0.10193679918450561</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -791,10 +798,10 @@
         <v>31</v>
       </c>
       <c r="B19" s="8">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C19" s="7">
-        <v>2.90519877675841</v>
+        <v>2.8032619775739041</v>
       </c>
     </row>
     <row r="20">
@@ -1075,43 +1082,43 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B4">
-        <v>6481537819.878829</v>
+        <v>2042580.7753590087</v>
       </c>
       <c r="C4">
-        <v>333333.34375</v>
+        <v>251904.90625</v>
       </c>
       <c r="D4">
-        <v>700000</v>
+        <v>453428.84375</v>
       </c>
       <c r="E4">
-        <v>1500000</v>
+        <v>1007619.5625</v>
       </c>
       <c r="F4">
-        <v>3229734.5</v>
+        <v>2657232.5</v>
       </c>
       <c r="G4">
-        <v>6000000</v>
+        <v>4042826.125</v>
       </c>
       <c r="H4">
-        <v>4372125194.1933126</v>
+        <v>2059723.0191452242</v>
       </c>
       <c r="I4">
-        <v>416666.65625</v>
+        <v>251904.90625</v>
       </c>
       <c r="J4">
-        <v>794301.625</v>
+        <v>463618.8125</v>
       </c>
       <c r="K4">
-        <v>1634120.125</v>
+        <v>1007619.625</v>
       </c>
       <c r="L4">
-        <v>3303803.75</v>
+        <v>2653803.75</v>
       </c>
       <c r="M4">
-        <v>6025734.75</v>
+        <v>4168662</v>
       </c>
     </row>
   </sheetData>
@@ -1122,4 +1129,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:O4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>434219.62010040088</v>
+      </c>
+      <c r="C4">
+        <v>120914.3515625</v>
+      </c>
+      <c r="D4">
+        <v>201523.921875</v>
+      </c>
+      <c r="E4">
+        <v>300000</v>
+      </c>
+      <c r="F4">
+        <v>478619.3125</v>
+      </c>
+      <c r="G4">
+        <v>834161.9375</v>
+      </c>
+      <c r="H4">
+        <v>2687251.75</v>
+      </c>
+      <c r="I4">
+        <v>435681.67022345966</v>
+      </c>
+      <c r="J4">
+        <v>115507.0625</v>
+      </c>
+      <c r="K4">
+        <v>201523.921875</v>
+      </c>
+      <c r="L4">
+        <v>300000</v>
+      </c>
+      <c r="M4">
+        <v>490039.53125</v>
+      </c>
+      <c r="N4">
+        <v>850000</v>
+      </c>
+      <c r="O4">
+        <v>2683666.75</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>